<commit_message>
finish settting up final output file across all four demo cats
</commit_message>
<xml_diff>
--- a/RISE-2-Level-Strat-output_example.xlsx
+++ b/RISE-2-Level-Strat-output_example.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/TOD-R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640F6865-70C4-824E-9E9F-3B3A8A538F60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07807DBC-B718-9E4D-8392-A12F8EBA32EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D91B89C0-13C6-5644-99EE-0CE34BD162C0}"/>
+    <workbookView xWindow="25720" yWindow="0" windowWidth="25480" windowHeight="28800" activeTab="1" xr2:uid="{D91B89C0-13C6-5644-99EE-0CE34BD162C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Still needed 2-level strat" sheetId="1" r:id="rId1"/>
+    <sheet name="Var_names" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="39">
   <si>
     <t>PARENT</t>
   </si>
@@ -149,6 +150,27 @@
   </si>
   <si>
     <t>SELF</t>
+  </si>
+  <si>
+    <t>_census_pct</t>
+  </si>
+  <si>
+    <t>_actual</t>
+  </si>
+  <si>
+    <t>_needed</t>
+  </si>
+  <si>
+    <t>No_HS_deg</t>
+  </si>
+  <si>
+    <t>HS_grad</t>
+  </si>
+  <si>
+    <t>Some_college</t>
+  </si>
+  <si>
+    <t>BA_plus</t>
   </si>
 </sst>
 </file>
@@ -756,31 +778,40 @@
     <xf numFmtId="1" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -810,46 +841,37 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1171,7 +1193,7 @@
   </sheetPr>
   <dimension ref="A1:AW54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="214" workbookViewId="0">
       <selection activeCell="AU4" sqref="AU4"/>
     </sheetView>
   </sheetViews>
@@ -1233,59 +1255,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="123" t="s">
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="126" t="s">
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
-      <c r="AA1" s="127"/>
-      <c r="AB1" s="127"/>
-      <c r="AC1" s="127"/>
-      <c r="AD1" s="127"/>
-      <c r="AE1" s="127"/>
-      <c r="AF1" s="127"/>
-      <c r="AG1" s="127"/>
-      <c r="AH1" s="127"/>
-      <c r="AI1" s="128"/>
-      <c r="AJ1" s="129" t="s">
+      <c r="V1" s="109"/>
+      <c r="W1" s="109"/>
+      <c r="X1" s="109"/>
+      <c r="Y1" s="109"/>
+      <c r="Z1" s="109"/>
+      <c r="AA1" s="109"/>
+      <c r="AB1" s="109"/>
+      <c r="AC1" s="109"/>
+      <c r="AD1" s="109"/>
+      <c r="AE1" s="109"/>
+      <c r="AF1" s="109"/>
+      <c r="AG1" s="109"/>
+      <c r="AH1" s="109"/>
+      <c r="AI1" s="110"/>
+      <c r="AJ1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="AK1" s="130"/>
-      <c r="AL1" s="130"/>
-      <c r="AM1" s="130"/>
-      <c r="AN1" s="130"/>
-      <c r="AO1" s="130"/>
-      <c r="AP1" s="130"/>
-      <c r="AQ1" s="130"/>
-      <c r="AR1" s="130"/>
-      <c r="AS1" s="130"/>
-      <c r="AT1" s="130"/>
-      <c r="AU1" s="131"/>
+      <c r="AK1" s="112"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
+      <c r="AN1" s="112"/>
+      <c r="AO1" s="112"/>
+      <c r="AP1" s="112"/>
+      <c r="AQ1" s="112"/>
+      <c r="AR1" s="112"/>
+      <c r="AS1" s="112"/>
+      <c r="AT1" s="112"/>
+      <c r="AU1" s="113"/>
       <c r="AV1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1297,81 +1319,81 @@
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="113" t="s">
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="115" t="s">
+      <c r="G2" s="115"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="118" t="s">
+      <c r="J2" s="119"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="116"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="118" t="s">
+      <c r="M2" s="119"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="118" t="s">
+      <c r="P2" s="119"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="106" t="s">
+      <c r="S2" s="119"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="108" t="s">
+      <c r="V2" s="128"/>
+      <c r="W2" s="128"/>
+      <c r="X2" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="108" t="s">
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="128"/>
+      <c r="AA2" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="107"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="108" t="s">
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="128"/>
+      <c r="AD2" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="107"/>
-      <c r="AF2" s="107"/>
-      <c r="AG2" s="108" t="s">
+      <c r="AE2" s="128"/>
+      <c r="AF2" s="128"/>
+      <c r="AG2" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="AH2" s="107"/>
-      <c r="AI2" s="109"/>
-      <c r="AJ2" s="110" t="s">
+      <c r="AH2" s="128"/>
+      <c r="AI2" s="130"/>
+      <c r="AJ2" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="103"/>
-      <c r="AL2" s="103"/>
-      <c r="AM2" s="102" t="s">
+      <c r="AK2" s="124"/>
+      <c r="AL2" s="124"/>
+      <c r="AM2" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="103"/>
-      <c r="AO2" s="104"/>
-      <c r="AP2" s="103" t="s">
+      <c r="AN2" s="124"/>
+      <c r="AO2" s="125"/>
+      <c r="AP2" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="AQ2" s="103"/>
-      <c r="AR2" s="103"/>
-      <c r="AS2" s="102" t="s">
+      <c r="AQ2" s="124"/>
+      <c r="AR2" s="124"/>
+      <c r="AS2" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="AT2" s="103"/>
-      <c r="AU2" s="105"/>
+      <c r="AT2" s="124"/>
+      <c r="AU2" s="126"/>
       <c r="AV2" s="7" t="s">
         <v>22</v>
       </c>
@@ -3046,59 +3068,59 @@
         <v>29</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="120" t="s">
+      <c r="C17" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="132"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="123" t="s">
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="124"/>
-      <c r="K17" s="124"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
-      <c r="R17" s="124"/>
-      <c r="S17" s="124"/>
-      <c r="T17" s="125"/>
-      <c r="U17" s="126" t="s">
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="106"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="106"/>
+      <c r="Q17" s="106"/>
+      <c r="R17" s="106"/>
+      <c r="S17" s="106"/>
+      <c r="T17" s="107"/>
+      <c r="U17" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="V17" s="127"/>
-      <c r="W17" s="127"/>
-      <c r="X17" s="127"/>
-      <c r="Y17" s="127"/>
-      <c r="Z17" s="127"/>
-      <c r="AA17" s="127"/>
-      <c r="AB17" s="127"/>
-      <c r="AC17" s="127"/>
-      <c r="AD17" s="127"/>
-      <c r="AE17" s="127"/>
-      <c r="AF17" s="127"/>
-      <c r="AG17" s="127"/>
-      <c r="AH17" s="127"/>
-      <c r="AI17" s="128"/>
-      <c r="AJ17" s="129" t="s">
+      <c r="V17" s="109"/>
+      <c r="W17" s="109"/>
+      <c r="X17" s="109"/>
+      <c r="Y17" s="109"/>
+      <c r="Z17" s="109"/>
+      <c r="AA17" s="109"/>
+      <c r="AB17" s="109"/>
+      <c r="AC17" s="109"/>
+      <c r="AD17" s="109"/>
+      <c r="AE17" s="109"/>
+      <c r="AF17" s="109"/>
+      <c r="AG17" s="109"/>
+      <c r="AH17" s="109"/>
+      <c r="AI17" s="110"/>
+      <c r="AJ17" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="AK17" s="130"/>
-      <c r="AL17" s="130"/>
-      <c r="AM17" s="130"/>
-      <c r="AN17" s="130"/>
-      <c r="AO17" s="130"/>
-      <c r="AP17" s="130"/>
-      <c r="AQ17" s="130"/>
-      <c r="AR17" s="130"/>
-      <c r="AS17" s="130"/>
-      <c r="AT17" s="130"/>
-      <c r="AU17" s="131"/>
+      <c r="AK17" s="112"/>
+      <c r="AL17" s="112"/>
+      <c r="AM17" s="112"/>
+      <c r="AN17" s="112"/>
+      <c r="AO17" s="112"/>
+      <c r="AP17" s="112"/>
+      <c r="AQ17" s="112"/>
+      <c r="AR17" s="112"/>
+      <c r="AS17" s="112"/>
+      <c r="AT17" s="112"/>
+      <c r="AU17" s="113"/>
       <c r="AV17" s="3" t="s">
         <v>5</v>
       </c>
@@ -3108,61 +3130,61 @@
     </row>
     <row r="18" spans="1:49">
       <c r="B18" s="6"/>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="113" t="s">
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="112"/>
-      <c r="H18" s="114"/>
-      <c r="U18" s="106" t="s">
+      <c r="G18" s="115"/>
+      <c r="H18" s="117"/>
+      <c r="U18" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="V18" s="107"/>
-      <c r="W18" s="107"/>
-      <c r="X18" s="108" t="s">
+      <c r="V18" s="128"/>
+      <c r="W18" s="128"/>
+      <c r="X18" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="Y18" s="107"/>
-      <c r="Z18" s="107"/>
-      <c r="AA18" s="108" t="s">
+      <c r="Y18" s="128"/>
+      <c r="Z18" s="128"/>
+      <c r="AA18" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="AB18" s="107"/>
-      <c r="AC18" s="107"/>
-      <c r="AD18" s="108" t="s">
+      <c r="AB18" s="128"/>
+      <c r="AC18" s="128"/>
+      <c r="AD18" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="AE18" s="107"/>
-      <c r="AF18" s="107"/>
-      <c r="AG18" s="108" t="s">
+      <c r="AE18" s="128"/>
+      <c r="AF18" s="128"/>
+      <c r="AG18" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="AH18" s="107"/>
-      <c r="AI18" s="109"/>
-      <c r="AJ18" s="110" t="s">
+      <c r="AH18" s="128"/>
+      <c r="AI18" s="130"/>
+      <c r="AJ18" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="AK18" s="103"/>
-      <c r="AL18" s="103"/>
-      <c r="AM18" s="102" t="s">
+      <c r="AK18" s="124"/>
+      <c r="AL18" s="124"/>
+      <c r="AM18" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="AN18" s="103"/>
-      <c r="AO18" s="104"/>
-      <c r="AP18" s="103" t="s">
+      <c r="AN18" s="124"/>
+      <c r="AO18" s="125"/>
+      <c r="AP18" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="AQ18" s="103"/>
-      <c r="AR18" s="103"/>
-      <c r="AS18" s="102" t="s">
+      <c r="AQ18" s="124"/>
+      <c r="AR18" s="124"/>
+      <c r="AS18" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="AT18" s="103"/>
-      <c r="AU18" s="105"/>
+      <c r="AT18" s="124"/>
+      <c r="AU18" s="126"/>
       <c r="AV18" s="7" t="s">
         <v>22</v>
       </c>
@@ -4558,59 +4580,59 @@
         <v>31</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="120" t="s">
+      <c r="C33" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="121"/>
-      <c r="E33" s="121"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="121"/>
-      <c r="H33" s="122"/>
-      <c r="I33" s="123" t="s">
+      <c r="D33" s="132"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="132"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="J33" s="124"/>
-      <c r="K33" s="124"/>
-      <c r="L33" s="124"/>
-      <c r="M33" s="124"/>
-      <c r="N33" s="124"/>
-      <c r="O33" s="124"/>
-      <c r="P33" s="124"/>
-      <c r="Q33" s="124"/>
-      <c r="R33" s="124"/>
-      <c r="S33" s="124"/>
-      <c r="T33" s="125"/>
-      <c r="U33" s="126" t="s">
+      <c r="J33" s="106"/>
+      <c r="K33" s="106"/>
+      <c r="L33" s="106"/>
+      <c r="M33" s="106"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="V33" s="127"/>
-      <c r="W33" s="127"/>
-      <c r="X33" s="127"/>
-      <c r="Y33" s="127"/>
-      <c r="Z33" s="127"/>
-      <c r="AA33" s="127"/>
-      <c r="AB33" s="127"/>
-      <c r="AC33" s="127"/>
-      <c r="AD33" s="127"/>
-      <c r="AE33" s="127"/>
-      <c r="AF33" s="127"/>
-      <c r="AG33" s="127"/>
-      <c r="AH33" s="127"/>
-      <c r="AI33" s="128"/>
-      <c r="AJ33" s="129" t="s">
+      <c r="V33" s="109"/>
+      <c r="W33" s="109"/>
+      <c r="X33" s="109"/>
+      <c r="Y33" s="109"/>
+      <c r="Z33" s="109"/>
+      <c r="AA33" s="109"/>
+      <c r="AB33" s="109"/>
+      <c r="AC33" s="109"/>
+      <c r="AD33" s="109"/>
+      <c r="AE33" s="109"/>
+      <c r="AF33" s="109"/>
+      <c r="AG33" s="109"/>
+      <c r="AH33" s="109"/>
+      <c r="AI33" s="110"/>
+      <c r="AJ33" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="AK33" s="130"/>
-      <c r="AL33" s="130"/>
-      <c r="AM33" s="130"/>
-      <c r="AN33" s="130"/>
-      <c r="AO33" s="130"/>
-      <c r="AP33" s="130"/>
-      <c r="AQ33" s="130"/>
-      <c r="AR33" s="130"/>
-      <c r="AS33" s="130"/>
-      <c r="AT33" s="130"/>
-      <c r="AU33" s="131"/>
+      <c r="AK33" s="112"/>
+      <c r="AL33" s="112"/>
+      <c r="AM33" s="112"/>
+      <c r="AN33" s="112"/>
+      <c r="AO33" s="112"/>
+      <c r="AP33" s="112"/>
+      <c r="AQ33" s="112"/>
+      <c r="AR33" s="112"/>
+      <c r="AS33" s="112"/>
+      <c r="AT33" s="112"/>
+      <c r="AU33" s="113"/>
       <c r="AV33" s="3" t="s">
         <v>5</v>
       </c>
@@ -4623,81 +4645,81 @@
         <v>23</v>
       </c>
       <c r="B34" s="6"/>
-      <c r="C34" s="111" t="s">
+      <c r="C34" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="113" t="s">
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="112"/>
-      <c r="H34" s="114"/>
-      <c r="I34" s="115" t="s">
+      <c r="G34" s="115"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J34" s="116"/>
-      <c r="K34" s="117"/>
-      <c r="L34" s="118" t="s">
+      <c r="J34" s="119"/>
+      <c r="K34" s="120"/>
+      <c r="L34" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="M34" s="116"/>
-      <c r="N34" s="117"/>
-      <c r="O34" s="118" t="s">
+      <c r="M34" s="119"/>
+      <c r="N34" s="120"/>
+      <c r="O34" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="117"/>
-      <c r="R34" s="118" t="s">
+      <c r="P34" s="119"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="S34" s="116"/>
-      <c r="T34" s="119"/>
-      <c r="U34" s="106" t="s">
+      <c r="S34" s="119"/>
+      <c r="T34" s="122"/>
+      <c r="U34" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="V34" s="107"/>
-      <c r="W34" s="107"/>
-      <c r="X34" s="108" t="s">
+      <c r="V34" s="128"/>
+      <c r="W34" s="128"/>
+      <c r="X34" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="Y34" s="107"/>
-      <c r="Z34" s="107"/>
-      <c r="AA34" s="108" t="s">
+      <c r="Y34" s="128"/>
+      <c r="Z34" s="128"/>
+      <c r="AA34" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="AB34" s="107"/>
-      <c r="AC34" s="107"/>
-      <c r="AD34" s="108" t="s">
+      <c r="AB34" s="128"/>
+      <c r="AC34" s="128"/>
+      <c r="AD34" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="AE34" s="107"/>
-      <c r="AF34" s="107"/>
-      <c r="AG34" s="108" t="s">
+      <c r="AE34" s="128"/>
+      <c r="AF34" s="128"/>
+      <c r="AG34" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="AH34" s="107"/>
-      <c r="AI34" s="109"/>
-      <c r="AJ34" s="110" t="s">
+      <c r="AH34" s="128"/>
+      <c r="AI34" s="130"/>
+      <c r="AJ34" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="AK34" s="103"/>
-      <c r="AL34" s="103"/>
-      <c r="AM34" s="102" t="s">
+      <c r="AK34" s="124"/>
+      <c r="AL34" s="124"/>
+      <c r="AM34" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="AN34" s="103"/>
-      <c r="AO34" s="104"/>
-      <c r="AP34" s="103" t="s">
+      <c r="AN34" s="124"/>
+      <c r="AO34" s="125"/>
+      <c r="AP34" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="AQ34" s="103"/>
-      <c r="AR34" s="103"/>
-      <c r="AS34" s="102" t="s">
+      <c r="AQ34" s="124"/>
+      <c r="AR34" s="124"/>
+      <c r="AS34" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="AT34" s="103"/>
-      <c r="AU34" s="105"/>
+      <c r="AT34" s="124"/>
+      <c r="AU34" s="126"/>
       <c r="AV34" s="7" t="s">
         <v>22</v>
       </c>
@@ -7397,6 +7419,46 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="AS34:AU34"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="X34:Z34"/>
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="AD34:AF34"/>
+    <mergeCell ref="AG34:AI34"/>
+    <mergeCell ref="AJ34:AL34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="AG18:AI18"/>
+    <mergeCell ref="AJ18:AL18"/>
+    <mergeCell ref="AM18:AO18"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AM34:AO34"/>
+    <mergeCell ref="AP34:AR34"/>
+    <mergeCell ref="AS18:AU18"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="I33:T33"/>
+    <mergeCell ref="U33:AI33"/>
+    <mergeCell ref="AJ33:AU33"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="AA18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:T17"/>
+    <mergeCell ref="U17:AI17"/>
+    <mergeCell ref="AJ17:AU17"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:T1"/>
     <mergeCell ref="U1:AI1"/>
@@ -7410,47 +7472,744 @@
     <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="AP2:AR2"/>
     <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:T17"/>
-    <mergeCell ref="U17:AI17"/>
-    <mergeCell ref="AJ17:AU17"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AS18:AU18"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="I33:T33"/>
-    <mergeCell ref="U33:AI33"/>
-    <mergeCell ref="AJ33:AU33"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="AA18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="AG18:AI18"/>
-    <mergeCell ref="AJ18:AL18"/>
-    <mergeCell ref="AM18:AO18"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="AM34:AO34"/>
-    <mergeCell ref="AP34:AR34"/>
-    <mergeCell ref="AS34:AU34"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="X34:Z34"/>
-    <mergeCell ref="AA34:AC34"/>
-    <mergeCell ref="AD34:AF34"/>
-    <mergeCell ref="AG34:AI34"/>
-    <mergeCell ref="AJ34:AL34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC305B98-C703-7C4B-82A4-F96E38DF21B9}">
+  <dimension ref="A1:B133"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>